<commit_message>
Update README.md and Data Overview files
</commit_message>
<xml_diff>
--- a/Data Overview 1.xlsx
+++ b/Data Overview 1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Esmaeil\irAEsProject\irAEsProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEA53A52-28DB-4ACF-B92F-50FCE9DEB190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA64349-AB7D-4CB4-9778-F4E2DD25EFA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{B9214421-C7AA-466F-926C-CBCB7BD6B19D}"/>
   </bookViews>
   <sheets>
     <sheet name="Part 1 (22 Samples)" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="139">
   <si>
     <t>"+CPI no colitis NC1"</t>
   </si>
@@ -453,6 +453,9 @@
   </si>
   <si>
     <t>Patients receiving Immune Checkpoint Inhibitors therapy who developed colitis</t>
+  </si>
+  <si>
+    <t>"+CPI colitis C6"</t>
   </si>
 </sst>
 </file>
@@ -869,7 +872,7 @@
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -954,7 +957,7 @@
         <v>121</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>138</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -962,12 +965,15 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -980,7 +986,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1128,8 +1134,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3038858-7A36-44C0-BC21-C5215BBD1362}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1414,7 +1420,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A6F10C5-3932-4272-A80F-198CD87810B3}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>

</xml_diff>